<commit_message>
updating, getting model H working
</commit_message>
<xml_diff>
--- a/data/ModelG_InternalCompound_Params.xlsx
+++ b/data/ModelG_InternalCompound_Params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steinanf/GitHub/TMDD_EndogenousLigand/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D44A6D6-20E5-4E4E-ADF2-4ACE7A7EB563}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B40FA1-3B8A-184B-A884-FD02618FD900}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12380" yWindow="900" windowWidth="17080" windowHeight="16900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4940" yWindow="960" windowWidth="17080" windowHeight="16900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1240,8 +1240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="C15" sqref="A15:XFD15"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>